<commit_message>
Test M002_Course Title creation
</commit_message>
<xml_diff>
--- a/TestData/TestExcelData.xlsx
+++ b/TestData/TestExcelData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NETCOM\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NETCOM\eclipse-workspace\MykademyLearningAPP\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01355E92-9FF9-4276-8D9B-08A18D74B33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C53699C-81E1-479A-A4EC-A305A8FB5B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{81580148-4C47-478B-8505-32CA94251ECD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -449,10 +449,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D31D20-265E-4C92-BB89-91B7665D7CAF}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,14 +468,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>